<commit_message>
Layout das exportações dos mapas
</commit_message>
<xml_diff>
--- a/IntegrationClient/Layout/Layout_Exportacao_LO.xlsx
+++ b/IntegrationClient/Layout/Layout_Exportacao_LO.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juremir.JMSOFT\Google Drive\FLUID State\Clientes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SystemCore\Manager\IntegrationClient\Layout\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE370BE3-E7ED-46FA-94A4-972FA210083F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{460EAD0C-B0B0-45B3-A42A-7CB95B39D600}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="782" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -654,6 +654,9 @@
     <xf numFmtId="0" fontId="27" fillId="21" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="10" xfId="42" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="25" fillId="22" borderId="11" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -674,9 +677,6 @@
     </xf>
     <xf numFmtId="0" fontId="27" fillId="21" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="10" xfId="42" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="60">
@@ -759,22 +759,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>32657</xdr:colOff>
+      <xdr:colOff>54429</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>54428</xdr:rowOff>
+      <xdr:rowOff>130628</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>478969</xdr:colOff>
+      <xdr:colOff>1018248</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>856557</xdr:rowOff>
+      <xdr:rowOff>740229</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Imagem 2">
+        <xdr:cNvPr id="4" name="Imagem 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C00C2DD4-B6C4-4AE3-89AC-C8E2E1393E78}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{57317C21-8AA4-4D81-9052-650291ABB523}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -796,8 +796,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="32657" y="54428"/>
-          <a:ext cx="2710541" cy="802129"/>
+          <a:off x="54429" y="130628"/>
+          <a:ext cx="3228048" cy="609601"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1160,7 +1160,7 @@
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection sqref="A1:J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1177,34 +1177,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="73.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
     </row>
     <row r="2" spans="1:10" ht="25.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
       <c r="H2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="13"/>
     </row>
     <row r="3" spans="1:10" ht="25.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="4"/>
@@ -1218,10 +1218,10 @@
       <c r="J3" s="4"/>
     </row>
     <row r="4" spans="1:10" ht="25.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="15"/>
+      <c r="B4" s="16"/>
       <c r="C4" s="8"/>
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
@@ -1232,28 +1232,28 @@
       <c r="J4" s="8"/>
     </row>
     <row r="5" spans="1:10" ht="25.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="9"/>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
-      <c r="J5" s="11"/>
+      <c r="A5" s="10"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="12"/>
     </row>
     <row r="6" spans="1:10" s="5" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6"/>
       <c r="B6" s="7"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="16"/>
-      <c r="I6" s="16"/>
-      <c r="J6" s="16"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>